<commit_message>
Tasks from P1-CIPL , P1-CL , P!-SS , P!-SI , P1-BL/AWB & P1-PEB_NPE
</commit_message>
<xml_diff>
--- a/Web/Content/EMCS/Templates/TemplateCatepillarSparePart.xlsx
+++ b/Web/Content/EMCS/Templates/TemplateCatepillarSparePart.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="68">
   <si>
     <t xml:space="preserve">ReferenceNo</t>
   </si>
@@ -71,31 +71,55 @@
     <t xml:space="preserve">Gross Weigth </t>
   </si>
   <si>
-    <t xml:space="preserve">1234J04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INJECTOR GP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11R0276</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J217</t>
-  </si>
-  <si>
-    <t xml:space="preserve">124.55</t>
+    <t xml:space="preserve">U-00001274</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INJ GP FUEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pcs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10R7224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">389.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1167.03</t>
   </si>
   <si>
     <t xml:space="preserve">USD</t>
   </si>
   <si>
-    <t xml:space="preserve">12345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carton Box</t>
+    <t xml:space="preserve">1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flexi Bag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COUPLING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1242131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87.20</t>
   </si>
   <si>
     <t xml:space="preserve">0.00</t>
@@ -107,58 +131,91 @@
     <t xml:space="preserve">0.000</t>
   </si>
   <si>
-    <t xml:space="preserve">1234H03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11R1130</t>
-  </si>
-  <si>
-    <t xml:space="preserve">112.87</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1244</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pcs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11R0272:AA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56.99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">227.96</t>
-  </si>
-  <si>
-    <t xml:space="preserve">345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11R0276:AA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">622.75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flexi Bag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11R0679</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74.16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">444.96</t>
+    <t xml:space="preserve">SUPPORT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1267521</t>
+  </si>
+  <si>
+    <t xml:space="preserve">285.31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">570.62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSERT THD R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1285113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">496.78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1987.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRIDGE A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1294181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">397.92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLIP-LOOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1345645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHAFT-TRACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1389712</t>
+  </si>
+  <si>
+    <t xml:space="preserve">309.97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEAR-OIL PUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1499110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">324.77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COUPLING AS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1530838</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">113.07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1530843</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74.76</t>
   </si>
 </sst>
 </file>
@@ -295,7 +352,7 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -311,94 +368,94 @@
         <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
         <v>23</v>
       </c>
       <c r="G3"/>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="L3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="O3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="P3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="Q3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="R3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="S3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4">
@@ -406,56 +463,56 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
         <v>23</v>
       </c>
       <c r="G4"/>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="L4" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="M4" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="N4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="O4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="P4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="Q4" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="R4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="S4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
@@ -463,56 +520,56 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
         <v>23</v>
       </c>
       <c r="G5"/>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="I5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="L5" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="M5" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="N5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="O5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="P5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="Q5" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="R5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="S5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6">
@@ -520,56 +577,341 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
         <v>23</v>
       </c>
       <c r="G6"/>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="L6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="M6" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="N6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>37</v>
+      </c>
+      <c r="R6" t="s">
+        <v>38</v>
+      </c>
+      <c r="S6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" t="s">
         <v>28</v>
       </c>
-      <c r="O6" t="s">
+      <c r="N7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>37</v>
+      </c>
+      <c r="R7" t="s">
+        <v>38</v>
+      </c>
+      <c r="S7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" t="s">
         <v>28</v>
       </c>
-      <c r="P6" t="s">
+      <c r="N8" t="s">
+        <v>36</v>
+      </c>
+      <c r="O8" t="s">
+        <v>36</v>
+      </c>
+      <c r="P8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>37</v>
+      </c>
+      <c r="R8" t="s">
+        <v>38</v>
+      </c>
+      <c r="S8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" t="s">
         <v>28</v>
       </c>
-      <c r="Q6" t="s">
-        <v>29</v>
-      </c>
-      <c r="R6" t="s">
-        <v>30</v>
-      </c>
-      <c r="S6" t="s">
-        <v>30</v>
+      <c r="N9" t="s">
+        <v>36</v>
+      </c>
+      <c r="O9" t="s">
+        <v>36</v>
+      </c>
+      <c r="P9" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>37</v>
+      </c>
+      <c r="R9" t="s">
+        <v>38</v>
+      </c>
+      <c r="S9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O10" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>37</v>
+      </c>
+      <c r="R10" t="s">
+        <v>38</v>
+      </c>
+      <c r="S10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" t="s">
+        <v>36</v>
+      </c>
+      <c r="O11" t="s">
+        <v>36</v>
+      </c>
+      <c r="P11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>37</v>
+      </c>
+      <c r="R11" t="s">
+        <v>38</v>
+      </c>
+      <c r="S11" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>